<commit_message>
Main changes, first draft done
</commit_message>
<xml_diff>
--- a/prodcat.xlsx
+++ b/prodcat.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kozh/Google Drive/Projects/Pricing models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kozh/Google Drive/Projects/Pricing models - GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="исж классический" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="62">
   <si>
     <t>und</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Депозит 2</t>
+  </si>
+  <si>
+    <t>memory</t>
   </si>
 </sst>
 </file>
@@ -690,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -800,7 +803,7 @@
         <v>29</v>
       </c>
       <c r="J3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -848,21 +851,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="33.83203125" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
     <col min="18" max="18" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -917,8 +921,11 @@
       <c r="R1" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2001</v>
       </c>
@@ -953,7 +960,7 @@
         <v>33</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -962,10 +969,13 @@
         <v>1E-3</v>
       </c>
       <c r="R2" s="5">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0.04</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2002</v>
       </c>
@@ -1011,8 +1021,11 @@
       <c r="R3" s="5">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2003</v>
       </c>
@@ -1061,8 +1074,11 @@
       <c r="R4" s="5">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2004</v>
       </c>
@@ -1114,11 +1130,14 @@
       <c r="R5" s="5">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I7" s="6"/>
     </row>
   </sheetData>
@@ -1359,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1407,7 +1426,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1427,7 +1446,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1447,7 +1466,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1460,7 +1479,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>